<commit_message>
jo/corrections to final automatization codes
</commit_message>
<xml_diff>
--- a/config/optimization_engine/config_optimization/ModelsML.xlsx
+++ b/config/optimization_engine/config_optimization/ModelsML.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="10305" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="10905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -40,12 +40,6 @@
     <t>process_b_y3</t>
   </si>
   <si>
-    <t>lr.pkl</t>
-  </si>
-  <si>
-    <t>custom</t>
-  </si>
-  <si>
     <t>PR_A</t>
   </si>
   <si>
@@ -65,6 +59,12 @@
   </si>
   <si>
     <t>PR_C_Y2</t>
+  </si>
+  <si>
+    <t>model.pkl</t>
+  </si>
+  <si>
+    <t>model.xlsx</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,58 +439,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>